<commit_message>
Added slides, updated examples
</commit_message>
<xml_diff>
--- a/Session 7 - Python/Instructional Material/Class Examples/Real World Loop Example/PartArrivalListener.xlsx
+++ b/Session 7 - Python/Instructional Material/Class Examples/Real World Loop Example/PartArrivalListener.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Repositories\PracticalProgramming\Session 7 - Python\Instructional Material\Class Examples\Real World Loop Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E183DC88-341E-4F43-9E7A-95C90CE956FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3865C918-80B1-4428-8DD1-D987293924C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="2175" windowWidth="15390" windowHeight="9532" xr2:uid="{C9622D37-428C-4E45-A6D8-FEE79D9DEC88}"/>
+    <workbookView xWindow="2040" yWindow="1583" windowWidth="15390" windowHeight="9532" xr2:uid="{C9622D37-428C-4E45-A6D8-FEE79D9DEC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated slides, worked on examples
</commit_message>
<xml_diff>
--- a/Session 7 - Python/Instructional Material/Class Examples/Real World Loop Example/PartArrivalListener.xlsx
+++ b/Session 7 - Python/Instructional Material/Class Examples/Real World Loop Example/PartArrivalListener.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Repositories\PracticalProgramming\Session 7 - Python\Instructional Material\Class Examples\Real World Loop Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3865C918-80B1-4428-8DD1-D987293924C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1269EE9-8A5C-46E3-B808-E08F18A1254B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1583" windowWidth="15390" windowHeight="9532" xr2:uid="{C9622D37-428C-4E45-A6D8-FEE79D9DEC88}"/>
+    <workbookView xWindow="4605" yWindow="1148" windowWidth="15390" windowHeight="9532" xr2:uid="{C9622D37-428C-4E45-A6D8-FEE79D9DEC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>